<commit_message>
#58532 For Excel cell formats with 3+ parts to them (eg +ve,-ve,0), which  DataFormatter didn't properly support, call out to the alternate CellFormat  instead for the formatting. This also allows us to enable some disabled parts of DataFormatter unit tests We still need to rationalise DataFormatter and CellFormatter though, so we  only have one set of cell formatting logic...
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1710399 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/FormatKM.xlsx
+++ b/test-data/spreadsheet/FormatKM.xlsx
@@ -16,18 +16,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>[&gt;999999]#,,"M";[&gt;999]#,"K";#</t>
   </si>
   <si>
     <t>[&gt;999999]#.000,,"M";[&gt;999]#.000,"K";#.000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>102K</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>10M</t>
+  </si>
+  <si>
+    <t>102M</t>
+  </si>
+  <si>
+    <t>1021M</t>
+  </si>
+  <si>
+    <t>1.020</t>
+  </si>
+  <si>
+    <t>10.200</t>
+  </si>
+  <si>
+    <t>102.102</t>
+  </si>
+  <si>
+    <t>1.021K</t>
+  </si>
+  <si>
+    <t>10.210K</t>
+  </si>
+  <si>
+    <t>102.102K</t>
+  </si>
+  <si>
+    <t>1.021M</t>
+  </si>
+  <si>
+    <t>102.102M</t>
+  </si>
+  <si>
+    <t>1021.021M</t>
+  </si>
+  <si>
+    <t>102.000</t>
+  </si>
+  <si>
+    <t>10.210M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[&gt;999999]#,,&quot;M&quot;;[&gt;999]#,&quot;K&quot;;#"/>
+    <numFmt numFmtId="165" formatCode="[&gt;999999]#.000,,&quot;M&quot;;[&gt;999]#.000,&quot;K&quot;;#.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,11 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,9 +444,10 @@
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -384,63 +455,221 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <f>A2</f>
+        <v>1.02</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <f>A2</f>
+        <v>1.02</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:B12" si="0">A3</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D12" si="1">A3</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>102.102</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>102.102</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="1"/>
+        <v>102.102</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1021.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>1021.02</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="1"/>
+        <v>1021.02</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10210.200000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>10210.200000000001</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="1"/>
+        <v>10210.200000000001</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>102102.102</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>102102.102</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>102102.102</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1021021.02</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>1021021.02</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>1021021.02</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10210210.199999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>10210210.199999999</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>10210210.199999999</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>102102102.102</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>102102102.102</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>102102102.102</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1021021021.02</v>
       </c>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>1021021021.02</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>1021021021.02</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2:C5 E2:E4 E5" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>